<commit_message>
fixed some graphics and queries
</commit_message>
<xml_diff>
--- a/exports/music_report.xlsx
+++ b/exports/music_report.xlsx
@@ -15,12 +15,12 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="q6" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'q1'!$A$1:$B$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'q1'!$A$1:$C$25</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'q2'!$A$1:$C$11</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'q3'!$A$1:$B$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'q3'!$A$1:$B$26</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'q4'!$A$1:$B$6</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'q5'!$A$1:$B$25</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'q6'!$A$1:$E$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'q6'!$A$1:$E$23</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -437,7 +437,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -450,6 +450,7 @@
   <cols>
     <col width="20" customWidth="1" min="1" max="1"/>
     <col width="13" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -463,6 +464,11 @@
           <t>tracks_sold</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>percentage</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -471,7 +477,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>837</v>
+        <v>838</v>
+      </c>
+      <c r="C2" t="n">
+        <v>37.36067766384307</v>
       </c>
     </row>
     <row r="3">
@@ -483,6 +492,9 @@
       <c r="B3" t="n">
         <v>386</v>
       </c>
+      <c r="C3" t="n">
+        <v>17.20909496210432</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -493,6 +505,9 @@
       <c r="B4" t="n">
         <v>264</v>
       </c>
+      <c r="C4" t="n">
+        <v>11.76995095853767</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -503,6 +518,9 @@
       <c r="B5" t="n">
         <v>244</v>
       </c>
+      <c r="C5" t="n">
+        <v>10.8782880071333</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -513,6 +531,9 @@
       <c r="B6" t="n">
         <v>80</v>
       </c>
+      <c r="C6" t="n">
+        <v>3.566651805617477</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -523,6 +544,9 @@
       <c r="B7" t="n">
         <v>61</v>
       </c>
+      <c r="C7" t="n">
+        <v>2.719572001783326</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -533,6 +557,9 @@
       <c r="B8" t="n">
         <v>47</v>
       </c>
+      <c r="C8" t="n">
+        <v>2.095407935800268</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -543,6 +570,9 @@
       <c r="B9" t="n">
         <v>41</v>
       </c>
+      <c r="C9" t="n">
+        <v>1.827909050378957</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -553,6 +583,9 @@
       <c r="B10" t="n">
         <v>41</v>
       </c>
+      <c r="C10" t="n">
+        <v>1.827909050378957</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -563,11 +596,208 @@
       <c r="B11" t="n">
         <v>30</v>
       </c>
+      <c r="C11" t="n">
+        <v>1.337494427106554</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Drama</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>29</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1.292911279536335</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Pop</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>28</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1.248328131966117</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Soundtrack</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>20</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.8916629514043692</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Sci Fi &amp; Fantasy</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>20</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.8916629514043692</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Hip Hop/Rap</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>17</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.7579135086937138</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Bossa Nova</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>15</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.6687472135532769</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Alternative</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>14</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.6241640659830584</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>World</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>13</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.57958091841284</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Heavy Metal</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>12</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.5349977708426215</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Electronica/Dance</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>12</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.5349977708426215</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Easy Listening</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>10</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0.4458314757021846</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Comedy</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>9</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.4012483281319661</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Rock And Roll</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>6</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.2674988854213107</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Science Fiction</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>6</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0.2674988854213107</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B11"/>
-  <conditionalFormatting sqref="B2:B11">
+  <autoFilter ref="A1:C25"/>
+  <conditionalFormatting sqref="B2:B25">
     <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFAA0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00AA00"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C25">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -633,7 +863,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>52.97</v>
+        <v>92.97</v>
       </c>
     </row>
     <row r="3">
@@ -795,7 +1025,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -915,16 +1145,166 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Hungary</t>
+          <t>Ireland</t>
         </is>
       </c>
       <c r="B11" t="n">
         <v>446.62</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Hungary</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>446.62</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Chile</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>415.62</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Austria</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>404.62</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Norway</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>362.62</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Netherlands</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>352.62</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Finland</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>350.62</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Sweden</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>340.62</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Australia</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>334.62</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Belgium</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>334.62</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Italy</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>334.62</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Denmark</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>334.62</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Spain</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>334.62</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Argentina</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>334.62</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Poland</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>334.62</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Kazakhstan</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>106</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:B11"/>
-  <conditionalFormatting sqref="B2:B11">
+  <autoFilter ref="A1:B26"/>
+  <conditionalFormatting sqref="B2:B26">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -994,7 +1374,7 @@
         <v>2023</v>
       </c>
       <c r="B4" t="n">
-        <v>469.58</v>
+        <v>509.58</v>
       </c>
     </row>
     <row r="5">
@@ -1328,7 +1708,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -1376,205 +1756,205 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Ruslan Tuleuov</t>
+          <t>Helena Holý</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-10-12</t>
+          <t>2021-07-11</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-11-13</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>66</v>
+        <v>49.62</v>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>1586</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Helena Holý</t>
+          <t>Hugh O'Reilly</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2021-07-11</t>
+          <t>2021-02-03</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2025-11-13</t>
+          <t>2025-11-04</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>49.62</v>
+        <v>45.62</v>
       </c>
       <c r="E3" t="n">
-        <v>1586</v>
+        <v>1735</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Richard Cunningham</t>
+          <t>Fynn Zimmermann</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2021-11-07</t>
+          <t>2021-01-19</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2025-06-03</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>47.62</v>
+        <v>43.62</v>
       </c>
       <c r="E4" t="n">
-        <v>1245</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Luis Rojas</t>
+          <t>Victor Stevens</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2021-04-04</t>
+          <t>2021-03-06</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2024-10-14</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>46.62</v>
+        <v>42.62</v>
       </c>
       <c r="E5" t="n">
-        <v>1289</v>
+        <v>1735</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Ladislav Kovács</t>
+          <t>Terhi Hämäläinen</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2022-01-08</t>
+          <t>2021-08-11</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2025-07-20</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>45.62</v>
+        <v>41.62</v>
       </c>
       <c r="E6" t="n">
-        <v>1289</v>
+        <v>1586</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Hugh O'Reilly</t>
+          <t>Johannes Van der Berg</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2021-02-03</t>
+          <t>2021-05-10</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2025-11-04</t>
+          <t>2025-09-12</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>45.62</v>
+        <v>40.62</v>
       </c>
       <c r="E7" t="n">
-        <v>1735</v>
+        <v>1586</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Frank Ralston</t>
+          <t>Wyatt Girard</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2022-02-08</t>
+          <t>2021-02-02</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2025-08-20</t>
+          <t>2025-11-03</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>43.62</v>
+        <v>39.62</v>
       </c>
       <c r="E8" t="n">
-        <v>1289</v>
+        <v>1735</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Julia Barnett</t>
+          <t>Bjørn Hansen</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2021-11-07</t>
+          <t>2021-01-02</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-10-03</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>43.62</v>
+        <v>39.62</v>
       </c>
       <c r="E9" t="n">
-        <v>1289</v>
+        <v>1735</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Fynn Zimmermann</t>
+          <t>Roberto Almeida</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2021-01-19</t>
+          <t>2021-05-23</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2025-06-03</t>
+          <t>2025-10-05</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>43.62</v>
+        <v>37.62</v>
       </c>
       <c r="E10" t="n">
         <v>1596</v>
@@ -1583,21 +1963,21 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Victor Stevens</t>
+          <t>Kathy Chase</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2021-03-06</t>
+          <t>2021-03-05</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>42.62</v>
+        <v>37.62</v>
       </c>
       <c r="E11" t="n">
         <v>1735</v>
@@ -1606,44 +1986,44 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Astrid Gruber</t>
+          <t>Ellie Sullivan</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2021-12-08</t>
+          <t>2021-04-22</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2025-06-19</t>
+          <t>2025-09-04</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>42.62</v>
+        <v>37.62</v>
       </c>
       <c r="E12" t="n">
-        <v>1289</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Terhi Hämäläinen</t>
+          <t>Patrick Gray</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2021-08-11</t>
+          <t>2021-06-10</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>41.62</v>
+        <v>37.62</v>
       </c>
       <c r="E13" t="n">
         <v>1586</v>
@@ -1652,190 +2032,236 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Johannes Van der Berg</t>
+          <t>John Gordon</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2021-05-10</t>
+          <t>2021-01-11</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>2025-09-12</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>40.62</v>
+        <v>37.62</v>
       </c>
       <c r="E14" t="n">
-        <v>1586</v>
+        <v>1788</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Isabelle Mercier</t>
+          <t>Robert Brown</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2022-01-08</t>
+          <t>2021-07-24</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>40.62</v>
+        <v>37.62</v>
       </c>
       <c r="E15" t="n">
-        <v>1245</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>František Wichterlová</t>
+          <t>Daan Peeters</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2021-12-08</t>
+          <t>2021-01-03</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2025-05-06</t>
+          <t>2025-10-04</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>40.62</v>
+        <v>37.62</v>
       </c>
       <c r="E16" t="n">
-        <v>1245</v>
+        <v>1735</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Bjørn Hansen</t>
+          <t>Steve Murray</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2021-01-02</t>
+          <t>2021-03-22</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>2025-10-03</t>
+          <t>2025-08-04</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>39.62</v>
+        <v>37.62</v>
       </c>
       <c r="E17" t="n">
-        <v>1735</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Dan Miller</t>
+          <t>Emma Jones</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2022-05-12</t>
+          <t>2021-02-06</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>2025-11-21</t>
+          <t>2025-06-11</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>39.62</v>
+        <v>37.62</v>
       </c>
       <c r="E18" t="n">
-        <v>1289</v>
+        <v>1586</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>François Tremblay</t>
+          <t>Eduardo Martins</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2022-03-11</t>
+          <t>2021-04-09</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>2025-09-20</t>
+          <t>2025-08-12</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>39.62</v>
+        <v>37.62</v>
       </c>
       <c r="E19" t="n">
-        <v>1289</v>
+        <v>1586</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Wyatt Girard</t>
+          <t>Martha Silk</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2021-02-02</t>
+          <t>2021-03-09</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>2025-11-03</t>
+          <t>2025-07-12</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>39.62</v>
+        <v>37.62</v>
       </c>
       <c r="E20" t="n">
-        <v>1735</v>
+        <v>1586</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Heather Leacock</t>
+          <t>Enrique Muñoz</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2022-02-08</t>
+          <t>2021-06-23</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>2025-07-07</t>
+          <t>2025-11-05</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>39.62</v>
+        <v>37.62</v>
       </c>
       <c r="E21" t="n">
-        <v>1245</v>
+        <v>1596</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Mark Philips</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>2021-01-06</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>2025-05-11</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>37.62</v>
+      </c>
+      <c r="E22" t="n">
+        <v>1586</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Frank Harris</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>2021-02-19</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>2025-07-04</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>37.62</v>
+      </c>
+      <c r="E23" t="n">
+        <v>1596</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E21"/>
-  <conditionalFormatting sqref="D2:D21">
+  <autoFilter ref="A1:E23"/>
+  <conditionalFormatting sqref="D2:D23">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -1847,7 +2273,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E21">
+  <conditionalFormatting sqref="E2:E23">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>